<commit_message>
update LED package and JTAG pins
</commit_message>
<xml_diff>
--- a/EntireBoard/BOM_v3.xlsx
+++ b/EntireBoard/BOM_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhiyangzhang/Desktop/NeuralRecorder/EntireBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664298B7-25A6-BE42-B657-487905E393F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C567358D-5A93-CE4C-B2C9-5DD048595DEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="460" windowWidth="22720" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10480" yWindow="460" windowWidth="15120" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1930,15 +1930,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFC25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
final (??) board v3
</commit_message>
<xml_diff>
--- a/EntireBoard/BOM_v3.xlsx
+++ b/EntireBoard/BOM_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhiyangzhang/Desktop/NeuralRecorder/EntireBoard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\NeuralRecorder\EntireBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C567358D-5A93-CE4C-B2C9-5DD048595DEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4C00FE-58E3-42FE-B6E0-B9DB30189413}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="460" windowWidth="15120" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="1720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -413,6 +413,15 @@
   <si>
     <t>https://www.mouser.com/ProductDetail/TDK/MLF1608E6R8JT000?qs=sGAEpiMZZMsg%252By3WlYCkU4Ucsz4Og40l7%252BEG7%2FjXYxQ%3D</t>
   </si>
+  <si>
+    <t>intan chip!!!</t>
+  </si>
+  <si>
+    <t>cc2652</t>
+  </si>
+  <si>
+    <t>linear regulator</t>
+  </si>
 </sst>
 </file>
 
@@ -496,7 +505,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +522,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -646,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -767,6 +788,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1928,14 +1956,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFC25"/>
+  <dimension ref="A1:XFC26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
@@ -1983,7 +2011,7 @@
       </c>
     </row>
     <row r="2" spans="1:16383" ht="46.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="70" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2044,7 +2072,7 @@
         <f t="shared" ref="I3:I23" si="0">G3*H3</f>
         <v>2.0499999999999998</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="49" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2079,7 +2107,7 @@
       </c>
     </row>
     <row r="5" spans="1:16383" ht="16.75" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="67" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2112,7 +2140,7 @@
       </c>
     </row>
     <row r="6" spans="1:16383" ht="16.75" customHeight="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="67" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2145,7 +2173,7 @@
       </c>
     </row>
     <row r="7" spans="1:16383" ht="17" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="64" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2178,7 +2206,7 @@
       </c>
     </row>
     <row r="8" spans="1:16383" ht="17" customHeight="1">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="66" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="41" t="s">
@@ -18584,7 +18612,7 @@
       <c r="XFC8" s="36"/>
     </row>
     <row r="9" spans="1:16383" ht="16.75" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="64" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="39" t="s">
@@ -18617,7 +18645,7 @@
       </c>
     </row>
     <row r="10" spans="1:16383" ht="17" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="67" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -18648,7 +18676,7 @@
       </c>
     </row>
     <row r="11" spans="1:16383" ht="17" customHeight="1">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="68" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -18681,7 +18709,7 @@
       </c>
     </row>
     <row r="12" spans="1:16383" ht="15.5" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="67" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -18774,7 +18802,7 @@
       </c>
     </row>
     <row r="15" spans="1:16383" ht="22.75" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="64" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="58" t="s">
@@ -18807,7 +18835,7 @@
       </c>
     </row>
     <row r="16" spans="1:16383" ht="22.75" customHeight="1">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="64" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="59" t="s">
@@ -18840,7 +18868,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="22.75" customHeight="1">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="64" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="60" t="s">
@@ -18873,7 +18901,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="22.75" customHeight="1">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="64" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="60" t="s">
@@ -18937,7 +18965,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="22.75" customHeight="1">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="64" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="61" t="s">
@@ -18970,7 +18998,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="22.75" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="65" t="s">
         <v>120</v>
       </c>
       <c r="B21" s="62">
@@ -19003,7 +19031,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.5" customHeight="1">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="65" t="s">
         <v>117</v>
       </c>
       <c r="B22" s="30" t="s">
@@ -19036,7 +19064,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="22.75" customHeight="1">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="64" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -19068,11 +19096,24 @@
         <v>60</v>
       </c>
     </row>
+    <row r="24" spans="1:10" ht="16.75" customHeight="1">
+      <c r="A24" s="69" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="25" spans="1:10" ht="16.75" customHeight="1">
+      <c r="A25" s="69" t="s">
+        <v>126</v>
+      </c>
       <c r="H25" s="47"/>
       <c r="I25" s="47">
         <f>SUM(I2:I23)</f>
         <v>41.050000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16.75" customHeight="1">
+      <c r="A26" s="69" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -19081,9 +19122,10 @@
     <hyperlink ref="J23" r:id="rId2" xr:uid="{57CB8F89-C7CF-7843-A5DB-7ED3EA02420B}"/>
     <hyperlink ref="J22" r:id="rId3" xr:uid="{1ECEA7CB-0E4C-814C-BF5B-BE164E396DFE}"/>
     <hyperlink ref="J13" r:id="rId4" xr:uid="{ED651FCB-F47E-854A-BA21-716568270F42}"/>
+    <hyperlink ref="J3" r:id="rId5" xr:uid="{E4495110-54B3-43A9-9A5F-FC14CD71C7E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>